<commit_message>
Separação da criação da malha (foi para o Function.py). Implementaçõa da analise analitica do Fluxo-Pressão.
</commit_message>
<xml_diff>
--- a/results/Simulador_Pressao-Pressao/pressao-pressao_analitico.xlsx
+++ b/results/Simulador_Pressao-Pressao/pressao-pressao_analitico.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Agora dá pra rodar com diferentes malhas para os métodos. Ainda não dá pra rodar pra várias malhas na mesma rodada!
</commit_message>
<xml_diff>
--- a/results/Simulador_Pressao-Pressao/pressao-pressao_analitico.xlsx
+++ b/results/Simulador_Pressao-Pressao/pressao-pressao_analitico.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15347,7 +15347,7 @@
         <v>17044807.7984793</v>
       </c>
       <c r="EI13" t="n">
-        <v>17028418.79222975</v>
+        <v>17028418.79222976</v>
       </c>
       <c r="EJ13" t="n">
         <v>17012109.54269157</v>
@@ -28257,7 +28257,7 @@
         <v>18999996.40952426</v>
       </c>
       <c r="M24" t="n">
-        <v>18999998.75886126</v>
+        <v>18999998.75886127</v>
       </c>
       <c r="N24" t="n">
         <v>19000003.1220114</v>
@@ -29486,7 +29486,7 @@
         <v>19000184.56837913</v>
       </c>
       <c r="T25" t="n">
-        <v>19000122.07552377</v>
+        <v>19000122.07552378</v>
       </c>
       <c r="U25" t="n">
         <v>19000080.64421222</v>
@@ -29516,7 +29516,7 @@
         <v>19000002.81787579</v>
       </c>
       <c r="AD25" t="n">
-        <v>19000001.84006597</v>
+        <v>19000001.84006598</v>
       </c>
       <c r="AE25" t="n">
         <v>19000001.19261802</v>
@@ -29804,7 +29804,7 @@
         <v>18964620.39118522</v>
       </c>
       <c r="DV25" t="n">
-        <v>18963260.60197247</v>
+        <v>18963260.60197248</v>
       </c>
       <c r="DW25" t="n">
         <v>18961870.66488168</v>
@@ -45547,7 +45547,7 @@
         <v>18999879.74859816</v>
       </c>
       <c r="EI38" t="n">
-        <v>18999870.62686045</v>
+        <v>18999870.62686044</v>
       </c>
       <c r="EJ38" t="n">
         <v>18999860.95832314</v>

</xml_diff>